<commit_message>
added stamp_label feature and now all pdf shipping labels are in one file
</commit_message>
<xml_diff>
--- a/app_cache/sparkleland_verykship_shipment.xlsx
+++ b/app_cache/sparkleland_verykship_shipment.xlsx
@@ -713,7 +713,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Morgan Brenneman</t>
+          <t>Lucy Padilla</t>
         </is>
       </c>
       <c r="P2" t="inlineStr"/>
@@ -729,19 +729,23 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>1261 W Country Mile Dr</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr"/>
+          <t>7900 Colony Cir S</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Apt 305</t>
+        </is>
+      </c>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Riverton</t>
+          <t>Tamarac</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>UT</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -751,7 +755,7 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>84065</t>
+          <t>33321</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
@@ -768,7 +772,7 @@
       <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>"Open Jump Ring"</t>
+          <t>"Gold Filled Beads"</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
@@ -778,7 +782,7 @@
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>28.00</t>
+          <t>16.00</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr"/>

</xml_diff>